<commit_message>
delete old results of non normalization
</commit_message>
<xml_diff>
--- a/experiment_results/AGGREGATION_ARITHMETIC_MEAN_NORMALIZATION_ALPHA_BETA/Debug/4wise/0.95_.xlsx
+++ b/experiment_results/AGGREGATION_ARITHMETIC_MEAN_NORMALIZATION_ALPHA_BETA/Debug/4wise/0.95_.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>MUTATED_PROJECT</t>
   </si>
@@ -52,16 +52,10 @@
     <t>FEATURE_SPACE</t>
   </si>
   <si>
-    <t>_MultipleBugs_.NOB_1.ID_264</t>
-  </si>
-  <si>
-    <t>Transaction.Transaction.12</t>
-  </si>
-  <si>
-    <t>_MultipleBugs_.NOB_1.ID_54</t>
-  </si>
-  <si>
-    <t>BankAccount.Account.31</t>
+    <t>_MultipleBugs_.NOB_1.ID_165</t>
+  </si>
+  <si>
+    <t>Empty.PL_Interface_impl.21</t>
   </si>
 </sst>
 </file>
@@ -393,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -445,78 +439,37 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>27</v>
+        <v>257</v>
       </c>
       <c r="F2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H2">
-        <v>79</v>
+        <v>440</v>
       </c>
       <c r="I2">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="J2">
-        <v>79</v>
+        <v>446</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L2">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="M2">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>-1</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>74</v>
-      </c>
-      <c r="I3">
-        <v>7</v>
-      </c>
-      <c r="J3">
-        <v>76</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
-      </c>
-      <c r="L3">
-        <v>36</v>
-      </c>
-      <c r="M3">
-        <v>76</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>